<commit_message>
Updated slides and sample
</commit_message>
<xml_diff>
--- a/Performance Comparison.xlsx
+++ b/Performance Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10923"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsuarez/Documents/GitHub/DotNet2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF71EBAC-4459-674B-92EF-B332747CD201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73EE26A-C59B-FB43-86AF-36775D8B40AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Visual Performance" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>HttpClient Performance</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>Templated Control</t>
+  </si>
+  <si>
+    <t>Controls Performance</t>
   </si>
 </sst>
 </file>
@@ -473,13 +473,13 @@
                   <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>208</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>214</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1510,7 +1510,7 @@
   <dimension ref="B1:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1526,25 +1526,25 @@
   <sheetData>
     <row r="1" spans="2:4" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>51</v>
@@ -1555,18 +1555,18 @@
     </row>
     <row r="5" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
         <v>57</v>
       </c>
       <c r="D5" s="3">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="7">
         <v>44</v>
@@ -1577,13 +1577,13 @@
     </row>
     <row r="7" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7">
         <v>58</v>
       </c>
       <c r="D7" s="7">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>